<commit_message>
negative information & realistic sensor
</commit_message>
<xml_diff>
--- a/mem_layout.xlsx
+++ b/mem_layout.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\Desktop\fastslam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1000C2D6-5730-410F-A7D2-C82B2F6607CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A868D3-9F2B-4709-BA2B-3451379C9A6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="204" windowWidth="23040" windowHeight="12204" xr2:uid="{EAE998F7-F03C-4D2D-8C2F-C017546771F2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{EAE998F7-F03C-4D2D-8C2F-C017546771F2}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
     <sheet name="List2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <t>x</t>
   </si>
@@ -67,9 +66,6 @@
     <t>max_landmarks</t>
   </si>
   <si>
-    <t>6 + 6 x n_landmarks</t>
-  </si>
-  <si>
     <t>Dist matrix</t>
   </si>
   <si>
@@ -80,6 +76,15 @@
   </si>
   <si>
     <t>n_landmarks x n_measurements measurements_idx</t>
+  </si>
+  <si>
+    <t>landmark_prob</t>
+  </si>
+  <si>
+    <t>1 x n_landmarks</t>
+  </si>
+  <si>
+    <t>6 + 7 x n_landmarks</t>
   </si>
 </sst>
 </file>
@@ -96,7 +101,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +156,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -241,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -282,6 +293,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -300,9 +319,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -312,14 +328,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -634,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78132F9-7C48-491F-8CCB-E94492BC2201}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -657,7 +671,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>0</v>
@@ -737,125 +751,147 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
-      <c r="B8" s="20"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="14"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="17"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
-      <c r="B9" s="20"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="14"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="17"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
-      <c r="B10" s="20"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="14"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="17"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="18"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
-      <c r="B11" s="20"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="14"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="17"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="18"/>
-      <c r="B12" s="20"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="14"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="17"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="18"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
-      <c r="B13" s="20"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="14"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="17"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="18"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="18"/>
-      <c r="B14" s="20"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="14"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="17"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="18"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="I15" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="15"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="17"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="19"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="19"/>
-      <c r="B17" s="20"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="15"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="17"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="19"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="19"/>
-      <c r="B18" s="20"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="15"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="17"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="19"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
-      <c r="B19" s="20"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="15"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="17"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="19"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="19"/>
-      <c r="B20" s="20"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="15"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="17"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="19"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="19"/>
-      <c r="B21" s="20"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="15"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="17"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="19"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
-      <c r="B22" s="20"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="15"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="17"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="19"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="19"/>
-      <c r="B23" s="20"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="16"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="17"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="20"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="16"/>
+      <c r="B25" s="17"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="16"/>
+      <c r="B26" s="17"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="16"/>
+      <c r="B27" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
     <mergeCell ref="I7:I14"/>
     <mergeCell ref="I15:I23"/>
     <mergeCell ref="A7:A14"/>
@@ -885,104 +921,104 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="14"/>
+      <c r="B2" s="17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="20" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="14"/>
+      <c r="B3" s="17"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="14"/>
+      <c r="B4" s="17"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="14"/>
+      <c r="B5" s="17"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="14"/>
+      <c r="B6" s="17"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="14"/>
+      <c r="B7" s="17"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="27"/>
+      <c r="B9" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="24"/>
-      <c r="B3" s="20"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="24"/>
-      <c r="B4" s="20"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
-      <c r="B5" s="20"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="24"/>
-      <c r="B6" s="20"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
-      <c r="B7" s="20"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="24"/>
-      <c r="B8" s="20"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
-      <c r="B9" s="20" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="27"/>
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="27"/>
+      <c r="B11" s="17"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="27"/>
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="27"/>
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="27"/>
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="27"/>
+      <c r="B15" s="17"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="28"/>
+      <c r="B16" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="20"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="25"/>
-      <c r="B11" s="20"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="25"/>
-      <c r="B12" s="20"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="25"/>
-      <c r="B13" s="20"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
-      <c r="B14" s="20"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
-      <c r="B15" s="20"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
-      <c r="B16" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="26"/>
-      <c r="B17" s="20"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="17"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="26"/>
-      <c r="B18" s="20"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="17"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
-      <c r="B19" s="20"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="17"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="26"/>
-      <c r="B20" s="20"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="17"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="26"/>
-      <c r="B21" s="20"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="17"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="26"/>
-      <c r="B22" s="20"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="17"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="27"/>
+      <c r="A23" s="15"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="27"/>
+      <c r="A24" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>